<commit_message>
Added comments to ManWolf and driverDFA. Created State-description file
</commit_message>
<xml_diff>
--- a/Lab2/State-Transition.xlsx
+++ b/Lab2/State-Transition.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark\Documents\CMPT-440\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark\Documents\CMPT-440\Lab2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="18">
   <si>
     <t>q0</t>
   </si>
@@ -71,10 +71,13 @@
     <t>n</t>
   </si>
   <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>!a</t>
+    <t>State Transition Table</t>
+  </si>
+  <si>
+    <t>q10 = Error State</t>
+  </si>
+  <si>
+    <t>q9 = Success State</t>
   </si>
 </sst>
 </file>
@@ -99,7 +102,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="9" tint="-0.499984740745262"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -125,10 +128,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,151 +421,218 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:K19"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="J2" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K2" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I3" t="s">
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="J3" t="s">
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
         <v>1</v>
       </c>
-      <c r="K3" t="s">
+      <c r="E3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I4" t="s">
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="4"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
         <v>1</v>
       </c>
-      <c r="J4" t="s">
+      <c r="C5" t="s">
         <v>3</v>
       </c>
-      <c r="K4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I5" t="s">
+      <c r="D5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
         <v>2</v>
       </c>
-      <c r="J5" t="s">
-        <v>2</v>
-      </c>
-      <c r="K5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I6" t="s">
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
         <v>3</v>
       </c>
-      <c r="J6" t="s">
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
         <v>3</v>
       </c>
-      <c r="K6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>10</v>
+      <c r="C9" t="s">
+        <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" t="s">
-        <v>0</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>3</v>
+        <v>7</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C12" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" t="s">
-        <v>4</v>
+      <c r="C12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>4</v>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>10</v>
@@ -561,116 +640,19 @@
       <c r="C13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D13" t="s">
-        <v>3</v>
-      </c>
-      <c r="E13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" t="s">
-        <v>5</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E19" s="1" t="s">
+      <c r="D13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G4:H4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>